<commit_message>
generate new sample Excel files with fake data, with base transaction keys
</commit_message>
<xml_diff>
--- a/data/sample/relius_demo_sample.xlsx
+++ b/data/sample/relius_demo_sample.xlsx
@@ -468,22 +468,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>419239990</t>
+          <t>182525755</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Megan</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Beck</t>
+          <t>Hall</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,60 +500,64 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>159638939</t>
+          <t>673043377</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Kristin</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rosario</t>
+          <t>Douglas</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1965-07-20</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>1970-11-29</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2019-12-16</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>790243695</t>
+          <t>412571510</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Brenda</t>
+          <t>Theresa</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Wilson</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1947-06-18</t>
+          <t>1965-07-20</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2018-11-02</t>
+          <t>2021-10-18</t>
         </is>
       </c>
     </row>
@@ -565,123 +569,119 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>638084244</t>
+          <t>605511979</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lauren</t>
+          <t>Dawn</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Anderson</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1974-08-28</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2012-02-26</t>
-        </is>
-      </c>
+          <t>2003-03-16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>460985531</t>
+          <t>596839385</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Benjamin</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Carlson</t>
+          <t>Snyder</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1971-08-15</t>
+          <t>1947-06-18</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-09-30</t>
+          <t>2018-11-02</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>809578276</t>
+          <t>759875909</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>Brittany</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Gallagher</t>
+          <t>Ruiz</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1988-04-27</t>
+          <t>1978-08-02</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2013-08-24</t>
+          <t>2011-09-15</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>335705803</t>
+          <t>123193387</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lisa</t>
+          <t>Levi</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Hardin</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1960-01-22</t>
+          <t>1974-08-28</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2020-05-07</t>
+          <t>2012-02-26</t>
         </is>
       </c>
     </row>
@@ -693,119 +693,123 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>252612042</t>
+          <t>828164931</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Malik</t>
+          <t>Lauren</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Martinez</t>
+          <t>Montoya</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1968-02-02</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>1992-08-31</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2011-12-13</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>992782873</t>
+          <t>159710067</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Christine</t>
+          <t>Tamara</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Odonnell</t>
+          <t>Swanson</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1952-02-09</t>
+          <t>1971-08-15</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2017-06-28</t>
+          <t>2023-09-30</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>568055939</t>
+          <t>677603894</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Abigail</t>
+          <t>Jamie</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Wagner</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1967-05-23</t>
+          <t>1963-03-30</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2016-04-08</t>
+          <t>2018-12-12</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>763216833</t>
+          <t>499345089</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Evan</t>
+          <t>Andrew</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Flynn</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1971-02-20</t>
+          <t>1988-04-27</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2012-01-27</t>
+          <t>2013-08-24</t>
         </is>
       </c>
     </row>
@@ -817,86 +821,86 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>222735390</t>
+          <t>943121665</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Angelica</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Hamilton</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1954-03-28</t>
+          <t>1957-12-16</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2014-02-07</t>
+          <t>2021-06-15</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>250281799</t>
+          <t>415943638</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Chad</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Gregory</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1997-07-22</t>
+          <t>1960-01-22</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2021-03-02</t>
+          <t>2020-05-07</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>249719794</t>
+          <t>153215337</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Jeffery</t>
+          <t>Stephen</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Woods</t>
+          <t>Rodgers</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1959-08-08</t>
+          <t>1993-12-01</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -904,187 +908,187 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>453599621</t>
+          <t>660734335</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Lawrence</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Gonzalez</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2003-01-06</t>
+          <t>2000-07-26</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-08-04</t>
+          <t>2016-05-20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>122562354</t>
+          <t>812610447</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Conrad</t>
+          <t>Barnes</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1942-07-11</t>
+          <t>1961-03-01</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2021-02-21</t>
+          <t>2011-11-23</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>254546995</t>
+          <t>807483983</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Jesus</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2003-09-11</t>
+          <t>1952-02-09</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2020-07-08</t>
+          <t>2017-06-28</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>213010199</t>
+          <t>191518845</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Margaret</t>
+          <t>Timothy</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Hall</t>
+          <t>Cohen</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1977-06-12</t>
+          <t>1980-12-09</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2014-02-27</t>
+          <t>2023-08-15</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>550450343</t>
+          <t>464357647</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Wayne</t>
+          <t>Kristen</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Hubbard</t>
+          <t>Douglas</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1948-06-03</t>
+          <t>1967-05-23</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2014-06-06</t>
+          <t>2016-04-08</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>320265278</t>
+          <t>197329676</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Lindsey</t>
+          <t>David</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Jensen</t>
+          <t>Phillips</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1999-09-14</t>
+          <t>1974-05-20</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
@@ -1092,184 +1096,188 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>753879463</t>
+          <t>598345769</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>Melissa</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Atkins</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1994-01-28</t>
+          <t>1984-01-25</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2012-09-16</t>
+          <t>2017-01-28</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>335414844</t>
+          <t>593462606</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Sean</t>
+          <t>Benjamin</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Pruitt</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1970-07-20</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
+          <t>1949-02-12</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2012-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>637594023</t>
+          <t>116340304</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Nicole</t>
+          <t>Alexa</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Hartman</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1992-04-10</t>
+          <t>1992-07-15</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2023-07-31</t>
+          <t>2013-03-27</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>985484610</t>
+          <t>809847956</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Snyder</t>
+          <t>Case</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1969-08-20</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
+          <t>1958-01-20</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2023-05-15</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>437425623</t>
+          <t>230512338</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Brittany</t>
+          <t>Lindsay</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Key</t>
+          <t>Sanchez</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1950-03-06</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>2012-10-05</t>
-        </is>
-      </c>
+          <t>1968-08-27</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>455838392</t>
+          <t>648889896</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Kathleen</t>
+          <t>Donna</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Hodges</t>
+          <t>Ramos</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1941-04-02</t>
+          <t>1997-07-22</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2016-08-23</t>
+          <t>2021-03-02</t>
         </is>
       </c>
     </row>
@@ -1281,119 +1289,123 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>147977314</t>
+          <t>878716203</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Tyler</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Serrano</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1943-12-08</t>
+          <t>1944-08-19</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2024-02-22</t>
+          <t>2012-04-17</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>405966519</t>
+          <t>446816002</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Eric</t>
+          <t>Meghan</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Kline</t>
+          <t>Porter</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1960-11-19</t>
+          <t>1959-08-08</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2011-08-03</t>
+          <t>2013-04-12</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>827630933</t>
+          <t>932273710</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>Blake</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Barron</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1999-10-25</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
+          <t>1971-06-21</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2024-04-27</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>147384545</t>
+          <t>367249438</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Stephanie</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Chavez</t>
+          <t>Carter</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1996-06-05</t>
+          <t>1999-10-20</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2014-04-08</t>
+          <t>2014-09-14</t>
         </is>
       </c>
     </row>
@@ -1405,27 +1417,27 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>126588434</t>
+          <t>118567292</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Erik</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Richardson</t>
+          <t>Garrison</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2005-06-09</t>
+          <t>1940-11-17</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>2010-07-29</t>
         </is>
       </c>
     </row>
@@ -1437,54 +1449,54 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>884261472</t>
+          <t>845750846</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Amanda</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Potter</t>
+          <t>Powell</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1980-05-31</t>
+          <t>1989-01-11</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2014-02-02</t>
+          <t>2018-04-17</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>758036274</t>
+          <t>230907977</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Brenda</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Moses</t>
+          <t>Leonard</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1981-06-15</t>
+          <t>2001-05-26</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
@@ -1497,183 +1509,187 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>672809098</t>
+          <t>842861599</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Terri</t>
+          <t>Nicole</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Cox</t>
+          <t>Anderson</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1987-01-21</t>
+          <t>2003-09-11</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2019-12-28</t>
+          <t>2020-07-08</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>254844602</t>
+          <t>628376696</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Kelsey</t>
+          <t>Kenneth</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Barrett</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1993-06-02</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr"/>
+          <t>1948-04-02</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2012-02-29</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>859662755</t>
+          <t>896915572</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Joshua</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Rodgers</t>
+          <t>Wells</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1974-08-15</t>
+          <t>1977-06-12</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2017-09-17</t>
+          <t>2014-02-27</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>325197935</t>
+          <t>575368651</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Stacey</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Morton</t>
+          <t>Daniels</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1961-02-27</t>
+          <t>1994-07-11</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-05-23</t>
+          <t>2013-06-19</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>277341819</t>
+          <t>589061532</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Richard</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Evans</t>
+          <t>Espinoza</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1972-04-27</t>
+          <t>1948-06-03</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2011-05-26</t>
+          <t>2014-06-06</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>100449985</t>
+          <t>888272020</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Christine</t>
+          <t>Brandon</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Lopez</t>
+          <t>Curtis</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1995-09-17</t>
+          <t>1973-02-15</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2012-06-08</t>
+          <t>2021-06-21</t>
         </is>
       </c>
     </row>
@@ -1685,59 +1701,59 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>854271769</t>
+          <t>876728627</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Rhonda</t>
+          <t>Priscilla</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Lambert</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1984-08-12</t>
+          <t>1999-09-14</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2019-12-18</t>
+          <t>2022-02-10</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>861168742</t>
+          <t>536524271</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Dustin</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Wilkerson</t>
+          <t>Cooley</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1984-03-19</t>
+          <t>1980-09-18</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2014-12-28</t>
+          <t>2022-04-16</t>
         </is>
       </c>
     </row>
@@ -1749,121 +1765,113 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>458175513</t>
+          <t>385923481</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Tiffany</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Acosta</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1944-05-12</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>2016-12-23</t>
-        </is>
-      </c>
+          <t>1951-12-01</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>149001127</t>
+          <t>683349990</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Traci</t>
+          <t>Jack</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Travis</t>
+          <t>Hale</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1999-08-02</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
+          <t>1974-03-23</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2014-04-21</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>210034027</t>
+          <t>768643684</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Gregory</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Robinson</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2004-03-14</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>2018-01-01</t>
-        </is>
-      </c>
+          <t>1970-07-20</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>826351373</t>
+          <t>260603635</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Katie</t>
+          <t>Kristi</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Schmidt</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1996-06-24</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>2020-02-10</t>
-        </is>
-      </c>
+          <t>1969-05-26</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1873,119 +1881,119 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>431914333</t>
+          <t>764006125</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Melanie</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Mccarty</t>
+          <t>Allen</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1997-06-02</t>
+          <t>1989-01-12</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2018-11-09</t>
+          <t>2021-11-17</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>993800813</t>
+          <t>460701992</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Wanda</t>
+          <t>Pamela</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Rosales</t>
+          <t>Campbell</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1942-01-30</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>2024-05-06</t>
-        </is>
-      </c>
+          <t>1999-09-30</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>934869440</t>
+          <t>869925053</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Neal</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1995-07-06</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
+          <t>1998-03-13</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2012-07-03</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>158735257</t>
+          <t>534570779</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Timothy</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Bridges</t>
+          <t>Duran</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1996-05-10</t>
+          <t>1969-08-20</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2013-09-21</t>
+          <t>2015-04-16</t>
         </is>
       </c>
     </row>
@@ -1997,57 +2005,61 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>429567973</t>
+          <t>696579537</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Kelly</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Howell</t>
+          <t>Gonzalez</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1971-06-16</t>
+          <t>1972-07-24</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2012-02-22</t>
+          <t>2012-04-24</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>684167411</t>
+          <t>692214146</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Randy</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1997-03-12</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr"/>
+          <t>1952-02-24</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2018-11-07</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2057,29 +2069,25 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>952255691</t>
+          <t>636241838</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Catherine</t>
+          <t>Cassidy</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Hubbard</t>
+          <t>Velasquez</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1960-04-09</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>2011-06-12</t>
-        </is>
-      </c>
+          <t>2005-12-17</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2089,57 +2097,57 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>959786471</t>
+          <t>760245486</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Kevin</t>
+          <t>Travis</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Hall</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1977-08-14</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>2022-02-28</t>
-        </is>
-      </c>
+          <t>1941-04-02</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>788836595</t>
+          <t>483174065</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Regina</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Proctor</t>
+          <t>Pineda</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1967-09-19</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr"/>
+          <t>1969-03-28</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2021-05-26</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2149,82 +2157,86 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>469047961</t>
+          <t>442797053</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Karen</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Rogers</t>
+          <t>Hall</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1947-05-22</t>
+          <t>1990-03-16</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2013-12-20</t>
+          <t>2010-11-23</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>912049799</t>
+          <t>841069963</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Kendra</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Watkins</t>
+          <t>Bauer</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1955-07-25</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr"/>
+          <t>2002-03-25</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2024-04-07</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>750542102</t>
+          <t>670273884</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Nicole</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Watts</t>
+          <t>Ramos</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1942-06-02</t>
+          <t>1994-07-22</t>
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
@@ -2232,123 +2244,119 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>564304373</t>
+          <t>454539137</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Amanda</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Peters</t>
+          <t>Shah</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1992-06-16</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>2018-04-22</t>
-        </is>
-      </c>
+          <t>1960-11-19</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>897608295</t>
+          <t>961774945</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Robinson</t>
+          <t>Dunn</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1999-04-26</t>
+          <t>1946-12-26</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2023-08-21</t>
+          <t>2012-05-08</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>592592168</t>
+          <t>310459177</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Laura</t>
+          <t>Debbie</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Henry</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1961-07-29</t>
+          <t>1999-01-15</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2015-10-20</t>
+          <t>2023-08-05</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>141642849</t>
+          <t>994498386</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>George</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1945-05-10</t>
+          <t>1982-05-26</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2356,124 +2364,124 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>523505806</t>
+          <t>512311059</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Jennifer</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Cuevas</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1978-05-06</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>2011-11-29</t>
-        </is>
-      </c>
+          <t>1998-08-04</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>269357982</t>
+          <t>457778981</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Kyle</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Parker</t>
+          <t>Castro</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1967-02-08</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr"/>
+          <t>1996-06-05</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>2014-04-08</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>192588092</t>
+          <t>940265780</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>Vincent</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Gutierrez</t>
+          <t>Villanueva</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1959-01-09</t>
+          <t>1966-09-04</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2015-11-25</t>
+          <t>2016-10-15</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>318561170</t>
+          <t>819603599</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Timothy</t>
+          <t>Morgan</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Ortiz</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1980-05-07</t>
+          <t>2005-06-09</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2010-12-21</t>
+          <t>2023-11-01</t>
         </is>
       </c>
     </row>
@@ -2485,121 +2493,117 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>531609871</t>
+          <t>440573705</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Deleon</t>
+          <t>Daniels</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1981-02-24</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>2013-05-13</t>
-        </is>
-      </c>
+          <t>1950-06-24</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>574583305</t>
+          <t>944463288</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Regina</t>
+          <t>Andrew</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Hurst</t>
+          <t>Bell</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1973-11-18</t>
+          <t>1964-04-16</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2024-10-25</t>
+          <t>2019-03-09</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>794529835</t>
+          <t>727747421</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Allen</t>
+          <t>Carlos</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Mcdowell</t>
+          <t>Burch</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1950-08-21</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>2010-08-21</t>
-        </is>
-      </c>
+          <t>1957-12-27</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>139523143</t>
+          <t>713662250</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Renee</t>
+          <t>Joshua</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Hicks</t>
+          <t>Martinez</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1942-05-01</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr"/>
+          <t>1962-12-13</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>2021-04-09</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2609,150 +2613,146 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>324640806</t>
+          <t>886157905</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Christine</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Deleon</t>
+          <t>Reed</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1978-01-22</t>
+          <t>1981-06-15</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2021-09-30</t>
+          <t>2018-10-13</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>671371728</t>
+          <t>977744762</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Kathy</t>
+          <t>Nicholas</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Mosley</t>
+          <t>Gonzalez</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1973-06-18</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>2012-09-06</t>
-        </is>
-      </c>
+          <t>2003-01-20</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>458718721</t>
+          <t>444318609</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Duncan</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1946-03-29</t>
+          <t>1987-01-21</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2011-09-26</t>
+          <t>2019-12-28</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>746612333</t>
+          <t>545615549</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Kimberly</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Buck</t>
+          <t>Barnes</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1974-09-16</t>
+          <t>2004-04-04</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2015-10-17</t>
+          <t>2015-06-10</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>794838273</t>
+          <t>173306784</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Gary</t>
+          <t>Wayne</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Clark</t>
+          <t>Gonzalez</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1959-08-22</t>
+          <t>1993-06-02</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
@@ -2760,130 +2760,122 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>362204151</t>
+          <t>393736929</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Cheryl</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Hartman</t>
+          <t>Jenkins</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1954-05-07</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>2023-10-05</t>
-        </is>
-      </c>
+          <t>1990-12-15</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>615287323</t>
+          <t>264182284</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Andrew</t>
+          <t>Jesse</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Rose</t>
+          <t>Palmer</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1996-03-12</t>
+          <t>1956-07-21</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2017-07-10</t>
+          <t>2017-11-13</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>673682707</t>
+          <t>410197613</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Brandon</t>
+          <t>Kelly</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Rogers</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1948-10-27</t>
+          <t>1973-12-08</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2014-01-10</t>
+          <t>2014-03-08</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>932124992</t>
+          <t>897690989</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>Aaron</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Snow</t>
+          <t>Lowery</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1995-10-13</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>2013-11-05</t>
-        </is>
-      </c>
+          <t>1988-10-01</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2893,59 +2885,59 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>476438160</t>
+          <t>709220717</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Norman</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Espinoza</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1941-09-25</t>
+          <t>1961-02-27</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2021-05-23</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>995669470</t>
+          <t>237006457</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Christina</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Lawrence</t>
+          <t>Bell</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1982-06-05</t>
+          <t>1985-03-17</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2018-07-03</t>
+          <t>2022-02-13</t>
         </is>
       </c>
     </row>
@@ -2957,181 +2949,185 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>891734349</t>
+          <t>762413128</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Joshua</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Dorsey</t>
+          <t>Rhodes</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1979-06-11</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr"/>
+          <t>1972-04-27</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>2011-05-26</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>746964548</t>
+          <t>713500809</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Donna</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Lewis</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1995-01-09</t>
+          <t>1963-12-20</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2023-05-06</t>
+          <t>2014-07-02</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>597350017</t>
+          <t>436328815</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>Brent</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1974-12-21</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
+          <t>1995-09-17</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>731233350</t>
+          <t>297635151</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Elaine</t>
+          <t>Cathy</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Graham</t>
+          <t>Hanson</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2004-12-15</t>
+          <t>1950-09-17</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2022-06-21</t>
+          <t>2019-04-14</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>902210356</t>
+          <t>916174177</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Christine</t>
+          <t>Donald</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Hartman</t>
+          <t>Caldwell</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1949-08-17</t>
+          <t>1952-05-12</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2024-12-28</t>
+          <t>2020-02-21</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>822993214</t>
+          <t>559713672</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Tanya</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Dyer</t>
+          <t>Schmidt</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1947-07-18</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr"/>
+          <t>1983-11-01</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>2023-09-05</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3141,245 +3137,241 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>580037201</t>
+          <t>817633328</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Melanie</t>
+          <t>Amanda</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Escobar</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1941-07-07</t>
+          <t>1950-02-20</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2022-11-04</t>
+          <t>2020-01-18</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>159248239</t>
+          <t>273388188</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Murphy</t>
+          <t>Webb</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1997-07-16</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr"/>
+          <t>1961-12-15</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>2012-03-05</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>274339121</t>
+          <t>566823546</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Willis</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2002-07-31</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>2010-04-26</t>
-        </is>
-      </c>
+          <t>1998-05-19</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>479553610</t>
+          <t>906794868</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Kenneth</t>
+          <t>Jason</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Mcdowell</t>
+          <t>Long</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1949-07-01</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>2022-07-11</t>
-        </is>
-      </c>
+          <t>1944-05-12</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>804978788</t>
+          <t>583681629</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Gregory</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Barnes</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1977-10-13</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>2024-03-12</t>
-        </is>
-      </c>
+          <t>1970-09-14</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004PLAT</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>463199644</t>
+          <t>652135049</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Erin</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Lopez</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1951-12-19</t>
+          <t>2004-07-13</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2013-01-28</t>
+          <t>2012-11-10</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>300004PLAT</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>790483318</t>
+          <t>589074078</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Jeffrey</t>
+          <t>William</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Holt</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>1960-01-31</t>
+          <t>1999-08-02</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2022-07-02</t>
+          <t>2024-10-09</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>300004MBD</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>905360110</t>
+          <t>247836785</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Kelly</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Mendez</t>
+          <t>Mann</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1943-02-08</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr"/>
+          <t>2005-03-14</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>2024-08-03</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3389,22 +3381,22 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>399638366</t>
+          <t>275803672</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Tim</t>
+          <t>Mathew</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Edwards</t>
+          <t>Burgess</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1994-06-05</t>
+          <t>1975-03-20</t>
         </is>
       </c>
       <c r="F96" t="inlineStr"/>
@@ -3412,160 +3404,160 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>369071351</t>
+          <t>573768871</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Brittney</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Torres</t>
+          <t>Mitchell</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1998-10-21</t>
+          <t>1951-09-21</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2012-09-08</t>
+          <t>2013-04-02</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>400001ABC</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>220068654</t>
+          <t>328488441</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Jose</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Greene</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1954-11-22</t>
+          <t>1996-06-24</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2017-12-22</t>
+          <t>2020-02-10</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>300005R</t>
+          <t>300004MBDII</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>855629415</t>
+          <t>428964098</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Melissa</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Castillo</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2000-01-01</t>
+          <t>1990-07-30</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2017-12-21</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>300004MBDII</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>101858821</t>
+          <t>733954718</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Sara</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Rivas</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1956-03-16</t>
+          <t>1997-06-02</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2021-06-10</t>
+          <t>2018-11-09</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>400001ABC</t>
+          <t>300005R</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>684715252</t>
+          <t>445104402</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Hector</t>
+          <t>Tiffany</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Adams</t>
+          <t>Stewart</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1964-08-22</t>
+          <t>1995-12-21</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2022-09-19</t>
+          <t>2024-06-11</t>
         </is>
       </c>
     </row>

</xml_diff>